<commit_message>
Complete the ErrorCode define
Complete the ErrorCode define
</commit_message>
<xml_diff>
--- a/multi_DUT_SOP/Multi-DUT_ErrorCode.xlsx
+++ b/multi_DUT_SOP/Multi-DUT_ErrorCode.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="158">
   <si>
     <t>2GPR</t>
   </si>
@@ -38,20 +38,174 @@
     </r>
   </si>
   <si>
-    <t>CEXX, CMXX.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>此处</t>
+    <t>5GPR</t>
+  </si>
+  <si>
+    <t>DUT 5g PassPhrase is has a wrong format</t>
+  </si>
+  <si>
+    <r>
+      <t>5g</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>无线密码格式不正确</t>
+    </r>
+  </si>
+  <si>
+    <t>BDID</t>
+  </si>
+  <si>
+    <t>DUT Board ID not match</t>
+  </si>
+  <si>
+    <r>
+      <t>Board ID</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>不正确</t>
+    </r>
+  </si>
+  <si>
+    <t>SWTI</t>
+  </si>
+  <si>
+    <t>DUT SW Time not match</t>
+  </si>
+  <si>
+    <r>
+      <t>SW Time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>不正确</t>
+    </r>
+  </si>
+  <si>
+    <t>SNUM</t>
+  </si>
+  <si>
+    <t>Check Code in Factory Mode Failed</t>
+  </si>
+  <si>
+    <r>
+      <t>Serial Number</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>不正确</t>
+    </r>
+  </si>
+  <si>
+    <t>REVS</t>
+  </si>
+  <si>
+    <t>Incorrect release version</t>
+  </si>
+  <si>
+    <r>
+      <t>Release version</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>不正确</t>
+    </r>
+  </si>
+  <si>
+    <t>CFVS</t>
+  </si>
+  <si>
+    <t>Incorrect CFE version</t>
+  </si>
+  <si>
+    <r>
+      <t>CFE version</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>不正确</t>
+    </r>
+  </si>
+  <si>
+    <t>LMAC</t>
+  </si>
+  <si>
+    <t>DUT LAN MAC not match</t>
+  </si>
+  <si>
+    <r>
+      <t>MAC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>地址不正确</t>
+    </r>
+  </si>
+  <si>
+    <t>PINN</t>
+  </si>
+  <si>
+    <t>DUT PIN number not match</t>
+  </si>
+  <si>
+    <r>
+      <t>PIN Number</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>不正确</t>
+    </r>
+  </si>
+  <si>
+    <t>ROIF</t>
+  </si>
+  <si>
+    <t>Get Routerinfo fail</t>
+  </si>
+  <si>
+    <r>
+      <t>获得</t>
     </r>
     <r>
       <rPr>
@@ -61,16 +215,27 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>XX</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>表示两位数字，如</t>
+      <t>routerinfo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>失败</t>
+    </r>
+  </si>
+  <si>
+    <t>GIAL</t>
+  </si>
+  <si>
+    <t>DUT all is not gia link</t>
+  </si>
+  <si>
+    <r>
+      <t>网口连接失败或网口速率没有达到</t>
     </r>
     <r>
       <rPr>
@@ -80,16 +245,27 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>CE01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>，</t>
+      <t>1000M</t>
+    </r>
+  </si>
+  <si>
+    <t>2GSD</t>
+  </si>
+  <si>
+    <t>DUT 2g SSID not match</t>
+  </si>
+  <si>
+    <r>
+      <t>2g</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>无线</t>
     </r>
     <r>
       <rPr>
@@ -99,16 +275,36 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>表示</t>
+      <t>SSID</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>不正确</t>
+    </r>
+  </si>
+  <si>
+    <t>5GSD</t>
+  </si>
+  <si>
+    <t>DUT 5g SSID not match</t>
+  </si>
+  <si>
+    <r>
+      <t>5g</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>无线</t>
     </r>
     <r>
       <rPr>
@@ -118,30 +314,234 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>ambitconfig.txt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>中第一个测试项出错。</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">  CEXX</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>代表某个测试项在配置文件缺少必需的项目；</t>
+      <t>SSID</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>不正确</t>
+    </r>
+  </si>
+  <si>
+    <t>2GPP</t>
+  </si>
+  <si>
+    <t>DUT 2g Passphrase not match</t>
+  </si>
+  <si>
+    <r>
+      <t>2g</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>无线密码不正确</t>
+    </r>
+  </si>
+  <si>
+    <t>5GPP</t>
+  </si>
+  <si>
+    <t>DUT 5g Passphrase not match</t>
+  </si>
+  <si>
+    <r>
+      <t>5g</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>无线密码不正确</t>
+    </r>
+  </si>
+  <si>
+    <t>SKUN</t>
+  </si>
+  <si>
+    <t>DUT Sku not match</t>
+  </si>
+  <si>
+    <t>国别不正确</t>
+  </si>
+  <si>
+    <t>RNOR</t>
+  </si>
+  <si>
+    <t>Set router in status "reset no reboot" fail</t>
+  </si>
+  <si>
+    <t>设置按键测试模式失败</t>
+  </si>
+  <si>
+    <t>REBN</t>
+  </si>
+  <si>
+    <t>Not push Reset button or Reset button bad</t>
+  </si>
+  <si>
+    <r>
+      <t>Reset</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>按键失败</t>
+    </r>
+  </si>
+  <si>
+    <t>WFBN</t>
+  </si>
+  <si>
+    <t>Not push Wi-Fi button or button Wifi bad</t>
+  </si>
+  <si>
+    <r>
+      <t>Wi-Fi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>按键失败</t>
+    </r>
+  </si>
+  <si>
+    <t>WPBN</t>
+  </si>
+  <si>
+    <t>Not push WPS button or WPS button bad</t>
+  </si>
+  <si>
+    <r>
+      <t>WPS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>按键失败</t>
+    </r>
+  </si>
+  <si>
+    <t>LTL1</t>
+  </si>
+  <si>
+    <t>Lan1 connection fail</t>
+  </si>
+  <si>
+    <r>
+      <t>LAN2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>网口连接失败</t>
+    </r>
+  </si>
+  <si>
+    <t>LTL2</t>
+  </si>
+  <si>
+    <t>Lan2 connection fail</t>
+  </si>
+  <si>
+    <r>
+      <t>LAN3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>网口连接失败</t>
+    </r>
+  </si>
+  <si>
+    <t>LTL3</t>
+  </si>
+  <si>
+    <t>Lan3 connection fail</t>
+  </si>
+  <si>
+    <r>
+      <t>LAN4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>网口连接失败</t>
+    </r>
+  </si>
+  <si>
+    <t>PLTW</t>
+  </si>
+  <si>
+    <t>Wan connection fail</t>
+  </si>
+  <si>
+    <r>
+      <t>WAN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>网口连接失败</t>
+    </r>
+  </si>
+  <si>
+    <t>LWTP</t>
+  </si>
+  <si>
+    <t>LAN to WAN throughput is low</t>
+  </si>
+  <si>
+    <r>
+      <t>LAN1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>网口到</t>
     </r>
     <r>
       <rPr>
@@ -151,6 +551,692 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>WAN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>网口</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>thoughput</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>不合格</t>
+    </r>
+  </si>
+  <si>
+    <t>LDUP</t>
+  </si>
+  <si>
+    <t>Set LED on fail</t>
+  </si>
+  <si>
+    <t>设置所有灯全亮失败</t>
+  </si>
+  <si>
+    <t>LDPO</t>
+  </si>
+  <si>
+    <t>Power LED is not on</t>
+  </si>
+  <si>
+    <t>电源灯不显示绿色</t>
+  </si>
+  <si>
+    <t>LDWA</t>
+  </si>
+  <si>
+    <t>Wan LED is not green on</t>
+  </si>
+  <si>
+    <r>
+      <t>WAN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>网口指示灯不显示绿色</t>
+    </r>
+  </si>
+  <si>
+    <t>LD2G</t>
+  </si>
+  <si>
+    <t>2G Wireless LED is not on</t>
+  </si>
+  <si>
+    <r>
+      <t>2G</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>无线指示灯不显示绿色</t>
+    </r>
+  </si>
+  <si>
+    <t>LD5G</t>
+  </si>
+  <si>
+    <t>5G Wireless LED is not on</t>
+  </si>
+  <si>
+    <r>
+      <t>5G</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>无线指示灯不显示蓝色</t>
+    </r>
+  </si>
+  <si>
+    <t>LDL1</t>
+  </si>
+  <si>
+    <t>Lan1 LED is not on</t>
+  </si>
+  <si>
+    <r>
+      <t>LAN1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>网口指示灯不显示绿色</t>
+    </r>
+  </si>
+  <si>
+    <t>LDL2</t>
+  </si>
+  <si>
+    <t>Lan2 LED is not on</t>
+  </si>
+  <si>
+    <r>
+      <t>LAN2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>网口指示灯不显示绿色</t>
+    </r>
+  </si>
+  <si>
+    <t>LDL3</t>
+  </si>
+  <si>
+    <t>Lan3 LED is not on</t>
+  </si>
+  <si>
+    <r>
+      <t>LAN3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>网口指示灯不显示绿色</t>
+    </r>
+  </si>
+  <si>
+    <t>LDL4</t>
+  </si>
+  <si>
+    <t>Lan4 LED is not on</t>
+  </si>
+  <si>
+    <r>
+      <t>LAN4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>网口指示灯不显示绿色</t>
+    </r>
+  </si>
+  <si>
+    <t>LDU1</t>
+  </si>
+  <si>
+    <t>usb1 LED is not on</t>
+  </si>
+  <si>
+    <r>
+      <t>USB1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>指示灯不显示绿色</t>
+    </r>
+  </si>
+  <si>
+    <t>LDU2</t>
+  </si>
+  <si>
+    <t>usb2 LED is not on</t>
+  </si>
+  <si>
+    <r>
+      <t>USB2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>指示灯不显示绿色</t>
+    </r>
+  </si>
+  <si>
+    <t>LDWP</t>
+  </si>
+  <si>
+    <t>Wps LED is not on</t>
+  </si>
+  <si>
+    <r>
+      <t>WPS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>指示灯不显示绿色</t>
+    </r>
+  </si>
+  <si>
+    <t>LDDN</t>
+  </si>
+  <si>
+    <t>Set LED down fail</t>
+  </si>
+  <si>
+    <t>设置所有灯全灭失败</t>
+  </si>
+  <si>
+    <t>LWAN</t>
+  </si>
+  <si>
+    <t>WAN LED is not OK</t>
+  </si>
+  <si>
+    <r>
+      <t>设置</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WAN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>网口指示灯</t>
+    </r>
+  </si>
+  <si>
+    <t>LANG</t>
+  </si>
+  <si>
+    <t>DUT Language is not OK</t>
+  </si>
+  <si>
+    <r>
+      <t>语言包不正确</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>未升级</t>
+    </r>
+  </si>
+  <si>
+    <t>Wan LED is not amber on</t>
+  </si>
+  <si>
+    <r>
+      <t>WAN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>网口指示灯不显示橙色</t>
+    </r>
+  </si>
+  <si>
+    <t>USBA</t>
+  </si>
+  <si>
+    <t>Not found expected device</t>
+  </si>
+  <si>
+    <r>
+      <t>没有发现</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>USB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>连接</t>
+    </r>
+  </si>
+  <si>
+    <t>U1TP</t>
+  </si>
+  <si>
+    <t>USB1 throughput under spec</t>
+  </si>
+  <si>
+    <r>
+      <t>USB1 thoughput</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>测试不合格</t>
+    </r>
+  </si>
+  <si>
+    <t>U2TP</t>
+  </si>
+  <si>
+    <t>USB2 throughput under spec</t>
+  </si>
+  <si>
+    <r>
+      <t>USB2 thoughput</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>测试不合格</t>
+    </r>
+  </si>
+  <si>
+    <t>DFAU</t>
+  </si>
+  <si>
+    <t>Fail to set router default</t>
+  </si>
+  <si>
+    <r>
+      <t>设置产品</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>default</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>失败</t>
+    </r>
+  </si>
+  <si>
+    <t>PSTP</t>
+  </si>
+  <si>
+    <t>Fail to set POT stop</t>
+  </si>
+  <si>
+    <r>
+      <t>停止</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>POT Time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>失败</t>
+    </r>
+  </si>
+  <si>
+    <t>PERA</t>
+  </si>
+  <si>
+    <t>Fail to get DUT POT time</t>
+  </si>
+  <si>
+    <r>
+      <t>获得</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>POT Time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>失败</t>
+    </r>
+  </si>
+  <si>
+    <t>PTIM</t>
+  </si>
+  <si>
+    <t>Fail to erase DUT POT</t>
+  </si>
+  <si>
+    <r>
+      <t>清零</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>POT Time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>失败</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">NDUT    Can't connect to router   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>无法检测到产品。</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">NPAR    No Parser running in DUT    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>产品中</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Parser</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>没有打开，产品需重新设置。</t>
+    </r>
+  </si>
+  <si>
+    <t>CEXX, CMXX.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>此处</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>XX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>表示两位数字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CE01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>表示</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ambitconfig.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>中第一个测试项出错。</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  CEXX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>代表某个测试项在配置文件缺少必需的项目；</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>CMXX</t>
     </r>
     <r>
@@ -173,8 +1259,22 @@
     <t>Error 汉语描述</t>
   </si>
   <si>
-    <t>Multi-DUT 错误代码</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <t>Multi-DUT_WNDR4500_错误代码</t>
+  </si>
+  <si>
+    <t>LDS1</t>
+  </si>
+  <si>
+    <t>Symbol LED 1 is not on</t>
+  </si>
+  <si>
+    <t>"NETGEAR"標志燈不顯示白色</t>
+  </si>
+  <si>
+    <t>Symbol LED 2 is not on</t>
+  </si>
+  <si>
+    <t>LDS2</t>
   </si>
   <si>
     <t>Sample</t>
@@ -234,8 +1334,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -546,10 +1647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -561,21 +1662,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="A1" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>148</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>149</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
@@ -589,22 +1690,582 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A30" t="s">
+        <v>78</v>
+      </c>
+      <c r="B30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A31" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
+        <v>84</v>
+      </c>
+      <c r="B32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A33" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" t="s">
+        <v>88</v>
+      </c>
+      <c r="C33" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
+        <v>90</v>
+      </c>
+      <c r="B34" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
+        <v>93</v>
+      </c>
+      <c r="B35" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>96</v>
+      </c>
+      <c r="B36" t="s">
+        <v>97</v>
+      </c>
+      <c r="C36" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
+        <v>99</v>
+      </c>
+      <c r="B37" t="s">
+        <v>100</v>
+      </c>
+      <c r="C37" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A38" t="s">
+        <v>102</v>
+      </c>
+      <c r="B38" t="s">
+        <v>103</v>
+      </c>
+      <c r="C38" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A39" t="s">
+        <v>105</v>
+      </c>
+      <c r="B39" t="s">
+        <v>106</v>
+      </c>
+      <c r="C39" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A40" t="s">
+        <v>108</v>
+      </c>
+      <c r="B40" t="s">
+        <v>109</v>
+      </c>
+      <c r="C40" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A41" t="s">
+        <v>152</v>
+      </c>
+      <c r="B41" t="s">
+        <v>153</v>
+      </c>
+      <c r="C41" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A42" t="s">
+        <v>156</v>
+      </c>
+      <c r="B42" t="s">
+        <v>155</v>
+      </c>
+      <c r="C42" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A43" t="s">
+        <v>111</v>
+      </c>
+      <c r="B43" t="s">
+        <v>112</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A44" t="s">
+        <v>114</v>
+      </c>
+      <c r="B44" t="s">
+        <v>115</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A45" t="s">
+        <v>117</v>
+      </c>
+      <c r="B45" t="s">
+        <v>118</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A46" t="s">
+        <v>81</v>
+      </c>
+      <c r="B46" t="s">
+        <v>120</v>
+      </c>
+      <c r="C46" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A47" t="s">
+        <v>122</v>
+      </c>
+      <c r="B47" t="s">
+        <v>123</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A48" t="s">
+        <v>125</v>
+      </c>
+      <c r="B48" t="s">
+        <v>126</v>
+      </c>
+      <c r="C48" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A49" t="s">
+        <v>128</v>
+      </c>
+      <c r="B49" t="s">
+        <v>129</v>
+      </c>
+      <c r="C49" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A50" t="s">
+        <v>131</v>
+      </c>
+      <c r="B50" t="s">
+        <v>132</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A51" t="s">
+        <v>134</v>
+      </c>
+      <c r="B51" t="s">
+        <v>135</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A52" t="s">
+        <v>137</v>
+      </c>
+      <c r="B52" t="s">
+        <v>138</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A53" t="s">
+        <v>140</v>
+      </c>
+      <c r="B53" t="s">
+        <v>141</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A56" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A57" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A58" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A59" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A60" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change some error code define.
After the team review, change some error code define.
</commit_message>
<xml_diff>
--- a/multi_DUT_SOP/Multi-DUT_ErrorCode.xlsx
+++ b/multi_DUT_SOP/Multi-DUT_ErrorCode.xlsx
@@ -367,9 +367,6 @@
     </r>
   </si>
   <si>
-    <t>SKUN</t>
-  </si>
-  <si>
     <t>DUT Sku not match</t>
   </si>
   <si>
@@ -383,9 +380,6 @@
   </si>
   <si>
     <t>设置按键测试模式失败</t>
-  </si>
-  <si>
-    <t>REBN</t>
   </si>
   <si>
     <t>Not push Reset button or Reset button bad</t>
@@ -621,9 +615,6 @@
     </r>
   </si>
   <si>
-    <t>LD2G</t>
-  </si>
-  <si>
     <t>2G Wireless LED is not on</t>
   </si>
   <si>
@@ -701,9 +692,6 @@
     </r>
   </si>
   <si>
-    <t>LDL3</t>
-  </si>
-  <si>
     <t>Lan3 LED is not on</t>
   </si>
   <si>
@@ -779,9 +767,6 @@
       </rPr>
       <t>指示灯不显示绿色</t>
     </r>
-  </si>
-  <si>
-    <t>LDWP</t>
   </si>
   <si>
     <t>Wps LED is not on</t>
@@ -1047,9 +1032,6 @@
     </r>
   </si>
   <si>
-    <t>PTIM</t>
-  </si>
-  <si>
     <t>Fail to erase DUT POT</t>
   </si>
   <si>
@@ -1275,6 +1257,30 @@
   </si>
   <si>
     <t>LDS2</t>
+  </si>
+  <si>
+    <t>PTIN</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LWPS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LD2G</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LDL3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERBN</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKUM</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Sample</t>
@@ -1650,7 +1656,7 @@
   <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1663,20 +1669,20 @@
   <sheetData>
     <row r="1" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B2" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C2" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
@@ -1860,412 +1866,412 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
+        <v>156</v>
+      </c>
+      <c r="B19" t="s">
         <v>45</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
         <v>48</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
+        <v>155</v>
+      </c>
+      <c r="B21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" t="s">
         <v>51</v>
-      </c>
-      <c r="B21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" t="s">
         <v>54</v>
-      </c>
-      <c r="B22" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" t="s">
         <v>57</v>
-      </c>
-      <c r="B23" t="s">
-        <v>58</v>
-      </c>
-      <c r="C23" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" t="s">
         <v>60</v>
-      </c>
-      <c r="B24" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" t="s">
         <v>63</v>
-      </c>
-      <c r="B25" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" t="s">
         <v>66</v>
-      </c>
-      <c r="B26" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" t="s">
         <v>69</v>
-      </c>
-      <c r="B27" t="s">
-        <v>70</v>
-      </c>
-      <c r="C27" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" t="s">
         <v>72</v>
-      </c>
-      <c r="B28" t="s">
-        <v>73</v>
-      </c>
-      <c r="C28" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="B29" t="s">
-        <v>76</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="B30" t="s">
-        <v>79</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" t="s">
         <v>81</v>
-      </c>
-      <c r="B31" t="s">
-        <v>82</v>
-      </c>
-      <c r="C31" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>84</v>
+        <v>153</v>
       </c>
       <c r="B32" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C32" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B33" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C33" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B34" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C34" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B35" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C35" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>96</v>
+        <v>154</v>
       </c>
       <c r="B36" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C36" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B37" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C37" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B38" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C38" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B39" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C39" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>108</v>
+        <v>152</v>
       </c>
       <c r="B40" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C40" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B41" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C41" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B42" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C42" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B43" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B44" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B45" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B46" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C46" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B47" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B48" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C48" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B49" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C49" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B50" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B51" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B52" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="B53" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>